<commit_message>
BVT updated NGC-1345 and TC-55040
</commit_message>
<xml_diff>
--- a/Test Data/Build_Verification_Test.xlsx
+++ b/Test Data/Build_Verification_Test.xlsx
@@ -5,18 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\NGConsys\NGConsys Automation\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9024"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9024" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TC05_A" sheetId="1" r:id="rId1"/>
-    <sheet name="TC05_B" sheetId="3" r:id="rId2"/>
-    <sheet name="TC06" sheetId="4" r:id="rId3"/>
-    <sheet name="TC07_A" sheetId="7" r:id="rId4"/>
-    <sheet name="TC07_B" sheetId="6" r:id="rId5"/>
+    <sheet name="TC-14_Panel" sheetId="8" r:id="rId2"/>
+    <sheet name="TC-14_Device" sheetId="9" r:id="rId3"/>
+    <sheet name="TC05_B" sheetId="3" r:id="rId4"/>
+    <sheet name="TC06" sheetId="4" r:id="rId5"/>
+    <sheet name="TC07_A" sheetId="7" r:id="rId6"/>
+    <sheet name="TC07_B" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="50">
   <si>
     <t xml:space="preserve">Note: Do not change the column/rows index </t>
   </si>
@@ -100,13 +102,97 @@
   </si>
   <si>
     <t>LPBS 3000 - 9</t>
+  </si>
+  <si>
+    <t>Panel Name</t>
+  </si>
+  <si>
+    <t>Panel Node</t>
+  </si>
+  <si>
+    <t>CPU Type</t>
+  </si>
+  <si>
+    <t>Panel Type</t>
+  </si>
+  <si>
+    <t>Project Name Before Save</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Project name displayed after Saving</t>
+  </si>
+  <si>
+    <t>Pro32xD</t>
+  </si>
+  <si>
+    <t>MX1000</t>
+  </si>
+  <si>
+    <t>P485D</t>
+  </si>
+  <si>
+    <t>Node1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>CPU 801</t>
+  </si>
+  <si>
+    <t>PFI</t>
+  </si>
+  <si>
+    <t>FIM</t>
+  </si>
+  <si>
+    <t>Profile Consys *</t>
+  </si>
+  <si>
+    <t>testBVT15_1</t>
+  </si>
+  <si>
+    <t>testBVT15_2</t>
+  </si>
+  <si>
+    <t>testBVT15_3</t>
+  </si>
+  <si>
+    <t>Device Type</t>
+  </si>
+  <si>
+    <t>CP 830</t>
+  </si>
+  <si>
+    <t>Call Points</t>
+  </si>
+  <si>
+    <t>RIM 800</t>
+  </si>
+  <si>
+    <t>Ancillary</t>
+  </si>
+  <si>
+    <t>Profile Consys - C:\work\consys-uiauto\NGDesigner Saved Projects\testBVT15_1.pjd</t>
+  </si>
+  <si>
+    <t>Profile Consys - C:\work\consys-uiauto\NGDesigner Saved Projects\testBVT15_2.pjd</t>
+  </si>
+  <si>
+    <t>Profile Consys - C:\work\consys-uiauto\NGDesigner Saved Projects\testBVT15_3.pjd</t>
+  </si>
+  <si>
+    <t>Region Index(Loop A,B,C,D)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,8 +215,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +246,11 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -193,10 +291,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -233,8 +332,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -549,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,6 +780,236 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="72.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C5" s="1"/>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -780,7 +1112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -864,12 +1196,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -976,12 +1308,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,7 +1382,9 @@
       <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="5"/>
@@ -1064,6 +1398,9 @@
       </c>
       <c r="B8" s="4">
         <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated test data for BVT and TC_66
</commit_message>
<xml_diff>
--- a/Test Data/Build_Verification_Test.xlsx
+++ b/Test Data/Build_Verification_Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9024" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9024"/>
   </bookViews>
   <sheets>
     <sheet name="TC05_A" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
   <si>
     <t xml:space="preserve">Note: Do not change the column/rows index </t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>Detectors</t>
-  </si>
-  <si>
-    <t>LI800</t>
-  </si>
-  <si>
-    <t>Other</t>
   </si>
   <si>
     <t>801 PH</t>
@@ -326,14 +320,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -649,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,47 +660,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="21"/>
+      <c r="C2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="4"/>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -754,20 +748,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -798,47 +782,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="21"/>
+      <c r="C2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="4"/>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -849,94 +833,94 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="F7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -964,11 +948,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>41</v>
+      <c r="A1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -981,10 +965,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -996,11 +980,11 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>45</v>
+      <c r="A5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1030,47 +1014,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="21"/>
+      <c r="C2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="4"/>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1078,10 +1062,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
@@ -1128,62 +1112,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="21"/>
+      <c r="C2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="4"/>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1215,47 +1199,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="21"/>
+      <c r="C2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="4"/>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1280,7 +1264,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
@@ -1312,7 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1329,47 +1313,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="21"/>
+      <c r="C2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="4"/>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1377,13 +1361,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>

</xml_diff>

<commit_message>
Updated BVT test data
</commit_message>
<xml_diff>
--- a/Test Data/Build_Verification_Test.xlsx
+++ b/Test Data/Build_Verification_Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9024"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9024" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC05_A" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
   <si>
     <t xml:space="preserve">Note: Do not change the column/rows index </t>
   </si>
@@ -122,39 +122,18 @@
     <t>Pro32xD</t>
   </si>
   <si>
-    <t>MX1000</t>
-  </si>
-  <si>
-    <t>P485D</t>
-  </si>
-  <si>
     <t>Node1</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>CPU 801</t>
-  </si>
-  <si>
     <t>PFI</t>
   </si>
   <si>
-    <t>FIM</t>
-  </si>
-  <si>
-    <t>Profile Consys *</t>
-  </si>
-  <si>
     <t>testBVT15_1</t>
   </si>
   <si>
-    <t>testBVT15_2</t>
-  </si>
-  <si>
-    <t>testBVT15_3</t>
-  </si>
-  <si>
     <t>Device Type</t>
   </si>
   <si>
@@ -170,16 +149,13 @@
     <t>Ancillary</t>
   </si>
   <si>
-    <t>Profile Consys - C:\work\consys-uiauto\NGDesigner Saved Projects\testBVT15_1.pjd</t>
-  </si>
-  <si>
-    <t>Profile Consys - C:\work\consys-uiauto\NGDesigner Saved Projects\testBVT15_2.pjd</t>
-  </si>
-  <si>
-    <t>Profile Consys - C:\work\consys-uiauto\NGDesigner Saved Projects\testBVT15_3.pjd</t>
-  </si>
-  <si>
     <t>Region Index(Loop A,B,C,D)</t>
+  </si>
+  <si>
+    <t>Profile Consys * - 81.2.14.0</t>
+  </si>
+  <si>
+    <t>Profile Consys - C:\work\consys-uiauto\NGDesigner Saved Projects\testBVT15_1.pjd - 81.2.14.0</t>
   </si>
 </sst>
 </file>
@@ -645,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -765,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,7 +754,7 @@
     <col min="4" max="4" width="22.88671875" customWidth="1"/>
     <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="72.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="80.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -859,68 +835,22 @@
         <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="E8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -952,7 +882,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -965,10 +895,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -981,10 +911,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1367,7 +1297,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>

</xml_diff>